<commit_message>
Fix in lab4 MatProg
</commit_message>
<xml_diff>
--- a/MatProg/Lab4/Lab4.xlsx
+++ b/MatProg/Lab4/Lab4.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Labs\semester_5\MatProg\Lab4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Labs\semester_5\garbage\Lab4MatAdd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3619E7B3-1DD8-4E68-A49E-40F704B219DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F08948-80B9-4DBB-BAA4-07C796FE1BF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -464,7 +464,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -472,50 +472,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="60% — акцент3" xfId="2" builtinId="40"/>
@@ -545,8 +544,8 @@
       <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1021433" cy="481286"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -588,6 +587,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -690,7 +690,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -772,8 +772,8 @@
       <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="998350" cy="481286"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -815,6 +815,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -917,7 +918,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -1004,8 +1005,8 @@
       <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1021433" cy="481286"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -1047,6 +1048,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1149,7 +1151,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -1231,8 +1233,8 @@
       <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="998350" cy="481286"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -1274,6 +1276,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1376,7 +1379,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -1556,8 +1559,8 @@
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="424988" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -1629,19 +1632,7 @@
                         <a:rPr lang="en-US" sz="1100" b="0" i="1">
                           <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         </a:rPr>
-                        <m:t>1</m:t>
-                      </m:r>
-                      <m:r>
-                        <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>,</m:t>
-                      </m:r>
-                      <m:r>
-                        <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>3</m:t>
+                        <m:t>1,3</m:t>
                       </m:r>
                     </m:e>
                   </m:acc>
@@ -1652,7 +1643,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -1724,8 +1715,8 @@
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="424988" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -1797,19 +1788,7 @@
                         <a:rPr lang="en-US" sz="1100" b="0" i="1">
                           <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         </a:rPr>
-                        <m:t>1</m:t>
-                      </m:r>
-                      <m:r>
-                        <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>,</m:t>
-                      </m:r>
-                      <m:r>
-                        <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>3</m:t>
+                        <m:t>1,3</m:t>
                       </m:r>
                     </m:e>
                   </m:acc>
@@ -1820,7 +1799,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -2153,7 +2132,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2205,7 +2184,6 @@
       <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -2223,27 +2201,26 @@
       <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="4"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
@@ -2258,8 +2235,8 @@
       <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
@@ -2276,11 +2253,11 @@
       <c r="D9" s="2">
         <v>-9</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="15">
         <f>B9*$B$13+C9*$C$13+D9*$D$13</f>
         <v>-9.8999999999999986</v>
       </c>
-      <c r="F9" s="5"/>
+      <c r="F9" s="15"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
@@ -2297,11 +2274,11 @@
       <c r="D10" s="2">
         <v>-16</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="14">
         <f t="shared" ref="E10:E11" si="0">B10*$B$13+C10*$C$13+D10*$D$13</f>
         <v>-9.6999999999999993</v>
       </c>
-      <c r="F10" s="8"/>
+      <c r="F10" s="14"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
@@ -2318,11 +2295,11 @@
       <c r="D11" s="2">
         <v>-12</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="15">
         <f t="shared" si="0"/>
         <v>-12.15</v>
       </c>
-      <c r="F11" s="5"/>
+      <c r="F11" s="15"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
@@ -2370,24 +2347,24 @@
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
@@ -2402,8 +2379,8 @@
       <c r="D17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
@@ -2412,22 +2389,22 @@
         <v>0</v>
       </c>
       <c r="B18" s="2">
-        <f>B$12-B9</f>
+        <f t="shared" ref="B18:D20" si="2">B$12-B9</f>
         <v>1</v>
       </c>
       <c r="C18" s="2">
-        <f>C$12-C9</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="D18" s="2">
-        <f>D$12-D9</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="15">
         <f>B18*$B$21+C18*$C$21+D18*$D$21</f>
         <v>1.9499999999999997</v>
       </c>
-      <c r="F18" s="5"/>
+      <c r="F18" s="15"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
@@ -2436,44 +2413,44 @@
         <v>1</v>
       </c>
       <c r="B19" s="2">
-        <f>B$12-B10</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C19" s="2">
-        <f>C$12-C10</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D19" s="2">
-        <f>D$12-D10</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="E19" s="8">
-        <f t="shared" ref="E19:E20" si="2">B19*$B$21+C19*$C$21+D19*$D$21</f>
+      <c r="E19" s="14">
+        <f t="shared" ref="E19:E20" si="3">B19*$B$21+C19*$C$21+D19*$D$21</f>
         <v>1.75</v>
       </c>
-      <c r="F19" s="8"/>
+      <c r="F19" s="14"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B20" s="2">
-        <f>B$12-B11</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="C20" s="2">
-        <f>C$12-C11</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="D20" s="2">
-        <f>D$12-D11</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="E20" s="5">
-        <f t="shared" si="2"/>
+      <c r="E20" s="15">
+        <f t="shared" si="3"/>
         <v>4.2</v>
       </c>
-      <c r="F20" s="5"/>
+      <c r="F20" s="15"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -2490,22 +2467,18 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="E16:F17"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="A6:F6"/>
     <mergeCell ref="A23:F23"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="E9:F9"/>
@@ -2513,7 +2486,11 @@
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="E7:F8"/>
-    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="E16:F17"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="E20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2594,22 +2571,22 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
@@ -2622,8 +2599,8 @@
       <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -2638,11 +2615,11 @@
       <c r="D9" s="2">
         <v>-9</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="14">
         <f>B9*$B$13+C9*$C$13+D9*$D$13</f>
         <v>-9</v>
       </c>
-      <c r="F9" s="8"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -2657,11 +2634,11 @@
       <c r="D10" s="2">
         <v>-16</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="15">
         <f t="shared" ref="E10:E11" si="0">B10*$B$13+C10*$C$13+D10*$D$13</f>
         <v>-10</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="15"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -2676,11 +2653,11 @@
       <c r="D11" s="2">
         <v>-12</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="15">
         <f t="shared" si="0"/>
         <v>-14.333333333333332</v>
       </c>
-      <c r="F11" s="5"/>
+      <c r="F11" s="15"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -2729,22 +2706,22 @@
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
@@ -2757,74 +2734,74 @@
       <c r="D17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B18" s="2">
-        <f>B$12-B9</f>
+        <f t="shared" ref="B18:D20" si="3">B$12-B9</f>
         <v>1</v>
       </c>
       <c r="C18" s="2">
-        <f>C$12-C9</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="D18" s="2">
-        <f>D$12-D9</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="14">
         <f>B18*$B$21+C18*$C$21+D18*$D$21</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="F18" s="8"/>
+      <c r="F18" s="14"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="2">
-        <f>B$12-B10</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="C19" s="2">
-        <f>C$12-C10</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D19" s="2">
-        <f>D$12-D10</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="E19" s="5">
-        <f t="shared" ref="E19:E20" si="3">B19*$B$21+C19*$C$21+D19*$D$21</f>
+      <c r="E19" s="15">
+        <f t="shared" ref="E19:E20" si="4">B19*$B$21+C19*$C$21+D19*$D$21</f>
         <v>2.333333333333333</v>
       </c>
-      <c r="F19" s="5"/>
+      <c r="F19" s="15"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B20" s="2">
-        <f>B$12-B11</f>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="C20" s="2">
-        <f>C$12-C11</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="D20" s="2">
-        <f>D$12-D11</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="E20" s="5">
-        <f t="shared" si="3"/>
+      <c r="E20" s="15">
+        <f t="shared" si="4"/>
         <v>6.666666666666667</v>
       </c>
-      <c r="F20" s="5"/>
+      <c r="F20" s="15"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -2835,28 +2812,34 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="C21" s="2">
-        <f t="shared" ref="C21:D21" si="4">1/3</f>
+        <f t="shared" ref="C21:D21" si="5">1/3</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="D21" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="E7:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
     <mergeCell ref="A23:F23"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="A16:D16"/>
@@ -2864,12 +2847,6 @@
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="E20:F20"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="E7:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2881,7 +2858,7 @@
   <dimension ref="A1:U35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2903,20 +2880,18 @@
       <c r="G1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -2937,20 +2912,18 @@
       <c r="G2" s="2">
         <v>0.5</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2968,21 +2941,18 @@
       <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="16"/>
+      <c r="U3" s="16"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -3000,63 +2970,56 @@
       <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="16"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
@@ -3075,23 +3038,22 @@
       <c r="F7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
+      <c r="H7" s="15"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="16"/>
+      <c r="U7" s="16"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -3106,7 +3068,7 @@
       <c r="D8" s="2">
         <v>-9</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="4">
         <f>MIN(B8:D8)</f>
         <v>-11</v>
       </c>
@@ -3114,24 +3076,23 @@
         <f>MAX(B8:D8)</f>
         <v>-7</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="14">
         <f>E8*$G$2+F8*(1-$G$2)</f>
         <v>-9</v>
       </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
+      <c r="H8" s="14"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="16"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -3150,28 +3111,27 @@
         <f t="shared" ref="E9:E10" si="0">MIN(B9:D9)</f>
         <v>-16</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="4">
         <f t="shared" ref="F9:F10" si="1">MAX(B9:D9)</f>
         <v>-6</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="15">
         <f t="shared" ref="G9:G10" si="2">E9*$G$2+F9*(1-$G$2)</f>
         <v>-11</v>
       </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
+      <c r="H9" s="15"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="16"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -3194,24 +3154,23 @@
         <f t="shared" si="1"/>
         <v>-10</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="15">
         <f t="shared" si="2"/>
         <v>-15.5</v>
       </c>
-      <c r="H10" s="5"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
+      <c r="H10" s="15"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="16"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -3233,43 +3192,42 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="16"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="16"/>
+      <c r="T13" s="16"/>
+      <c r="U13" s="16"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -3288,22 +3246,22 @@
       <c r="F14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="5"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-      <c r="S14" s="3"/>
-      <c r="T14" s="3"/>
-      <c r="U14" s="3"/>
+      <c r="H14" s="15"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="16"/>
+      <c r="T14" s="16"/>
+      <c r="U14" s="16"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -3321,7 +3279,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="3">
         <f>MAX(B15:D15)</f>
         <v>3</v>
       </c>
@@ -3329,23 +3287,23 @@
         <f>MIN(B15:D15)</f>
         <v>0</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="21">
         <f>$G$2*E15+(1-$G$2)*F15</f>
         <v>1.5</v>
       </c>
-      <c r="H15" s="7"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
-      <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
-      <c r="U15" s="3"/>
+      <c r="H15" s="21"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="16"/>
+      <c r="S15" s="16"/>
+      <c r="T15" s="16"/>
+      <c r="U15" s="16"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -3371,23 +3329,23 @@
         <f t="shared" ref="F16:F17" si="7">MIN(B16:D16)</f>
         <v>0</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="16">
         <f t="shared" ref="G16:G17" si="8">$G$2*E16+(1-$G$2)*F16</f>
         <v>3.5</v>
       </c>
-      <c r="H16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
+      <c r="H16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
+      <c r="T16" s="16"/>
+      <c r="U16" s="16"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
@@ -3413,225 +3371,218 @@
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="16">
         <f t="shared" si="8"/>
         <v>8.5</v>
       </c>
-      <c r="H17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-      <c r="S17" s="3"/>
-      <c r="T17" s="3"/>
-      <c r="U17" s="3"/>
+      <c r="H17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="16"/>
+      <c r="U17" s="16"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
-      <c r="T18" s="3"/>
-      <c r="U18" s="3"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="16"/>
+      <c r="S18" s="16"/>
+      <c r="T18" s="16"/>
+      <c r="U18" s="16"/>
     </row>
     <row r="19" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="16"/>
+      <c r="T19" s="16"/>
+      <c r="U19" s="16"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
-      <c r="U20" s="3"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="16"/>
+      <c r="T20" s="16"/>
+      <c r="U20" s="16"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
     </row>
     <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
     </row>
     <row r="30" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
+      <c r="A31" s="19"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
+      <c r="A33" s="20"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A35:H35"/>
-    <mergeCell ref="A19:H21"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="A24:H27"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="A30:H31"/>
-    <mergeCell ref="A32:H33"/>
     <mergeCell ref="J13:U20"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="A6:H6"/>
@@ -3644,6 +3595,13 @@
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="G9:H9"/>
+    <mergeCell ref="A35:H35"/>
+    <mergeCell ref="A19:H21"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A24:H27"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="A30:H31"/>
+    <mergeCell ref="A32:H33"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3656,7 +3614,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3672,13 +3630,13 @@
       <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3696,13 +3654,13 @@
       <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -3720,13 +3678,13 @@
       <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -3744,38 +3702,38 @@
       <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="G6" s="3" t="s">
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="G6" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
@@ -3795,27 +3753,27 @@
       </c>
       <c r="B8" s="2">
         <f>B2*B$14</f>
-        <v>0.20588235294117646</v>
+        <v>0.3333333333333332</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" ref="C8:D8" si="0">C2*C$14</f>
-        <v>0.37931034482758619</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>0.24324324324324326</v>
+        <v>0.42857142857142844</v>
       </c>
       <c r="E8" s="2">
         <f>SUM(B8:D8)</f>
-        <v>0.82843594101200591</v>
-      </c>
-      <c r="G8" s="3" t="s">
+        <v>0.76190476190476164</v>
+      </c>
+      <c r="G8" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -3823,27 +3781,27 @@
       </c>
       <c r="B9" s="2">
         <f>B3*B$14</f>
-        <v>0.1764705882352941</v>
+        <v>0.28571428571428559</v>
       </c>
       <c r="C9" s="2">
         <f t="shared" ref="C9:D9" si="1">C3*C$14</f>
-        <v>0.27586206896551724</v>
+        <v>0</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="1"/>
-        <v>0.43243243243243246</v>
+        <v>0.76190476190476164</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" ref="E9:E10" si="2">SUM(B9:D9)</f>
-        <v>0.88476508963324374</v>
-      </c>
-      <c r="G9" s="3" t="s">
+        <v>1.0476190476190472</v>
+      </c>
+      <c r="G9" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -3851,60 +3809,60 @@
       </c>
       <c r="B10" s="2">
         <f>B4*B$14</f>
-        <v>0.61764705882352944</v>
+        <v>0.99999999999999967</v>
       </c>
       <c r="C10" s="2">
         <f t="shared" ref="C10:D10" si="3">C4*C$14</f>
-        <v>0.34482758620689657</v>
+        <v>0</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="3"/>
-        <v>0.32432432432432434</v>
+        <v>0.57142857142857117</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" si="2"/>
-        <v>1.2867989693547504</v>
-      </c>
-      <c r="G10" s="3" t="s">
+        <v>1.5714285714285707</v>
+      </c>
+      <c r="G10" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <f>SUM(B8:B10)</f>
-        <v>1</v>
+        <v>1.6190476190476186</v>
       </c>
       <c r="C11" s="2">
         <f t="shared" ref="C11:D11" si="4">SUM(C8:C10)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="G11" s="3" t="s">
+        <v>1.7619047619047612</v>
+      </c>
+      <c r="G11" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E12" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -3923,30 +3881,30 @@
         <f>SUM(B13:D13)</f>
         <v>9.5238095238095247E-2</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B14" s="2">
-        <v>2.9411764705882353E-2</v>
+        <v>4.7619047619047603E-2</v>
       </c>
       <c r="C14" s="2">
-        <v>3.4482758620689655E-2</v>
+        <v>0</v>
       </c>
       <c r="D14" s="2">
-        <v>2.7027027027027029E-2</v>
+        <v>4.7619047619047603E-2</v>
       </c>
       <c r="E14" s="2">
         <f>SUM(B14:D14)</f>
-        <v>9.0921550353599029E-2</v>
+        <v>9.5238095238095205E-2</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -3964,60 +3922,60 @@
       </c>
       <c r="B17">
         <f>1/E14</f>
-        <v>10.998492613807658</v>
+        <v>10.500000000000004</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B18" s="13">
+      <c r="B18" s="5">
         <f>$B$16*B13</f>
         <v>0</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="5">
         <f t="shared" ref="C18:D18" si="5">$B$16*C13</f>
         <v>0.75000000000000022</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="5">
         <f t="shared" si="5"/>
         <v>0.24999999999999961</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="22">
+      <c r="B19" s="13">
         <f>$B$17*B14</f>
-        <v>0.32348507687669581</v>
-      </c>
-      <c r="C19" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="C19" s="13">
         <f t="shared" ref="C19:D19" si="6">$B$17*C14</f>
-        <v>0.37925836599336749</v>
-      </c>
-      <c r="D19" s="22">
+        <v>0</v>
+      </c>
+      <c r="D19" s="13">
         <f t="shared" si="6"/>
-        <v>0.2972565571299367</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="G5:K5"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="G9:K9"/>
     <mergeCell ref="G11:K11"/>
     <mergeCell ref="G12:K12"/>
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="A6:E6"/>
-    <mergeCell ref="G5:K5"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="G9:K9"/>
     <mergeCell ref="G10:K10"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="G2:K2"/>
-    <mergeCell ref="G3:K3"/>
-    <mergeCell ref="G4:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4029,7 +3987,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4045,17 +4003,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="6" t="s">
         <v>61</v>
       </c>
     </row>
@@ -4065,113 +4023,113 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18" t="s">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="9" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="10" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="7">
         <v>0</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="7">
         <v>-0.33333333333333331</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="7">
         <v>1</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="7">
         <v>0.33333333333333331</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="7">
         <v>1E+30</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="7">
         <v>7.1428571428571466E-2</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="7">
         <v>0</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="7">
         <v>1</v>
       </c>
-      <c r="G10" s="16">
+      <c r="G10" s="7">
         <v>0.13333333333333333</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10" s="7">
         <v>0.16666666666666669</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="8">
         <v>2.3809523809523777E-2</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="8">
         <v>0</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="8">
         <v>1</v>
       </c>
-      <c r="G11" s="17">
+      <c r="G11" s="8">
         <v>0.20000000000000004</v>
       </c>
-      <c r="H11" s="17">
+      <c r="H11" s="8">
         <v>8.6956521739130432E-2</v>
       </c>
     </row>
@@ -4181,113 +4139,113 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18" t="s">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="G14" s="18" t="s">
+      <c r="G14" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="9" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="F15" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="G15" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="H15" s="10" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="7">
         <v>1.0000000000000002</v>
       </c>
-      <c r="E16" s="20">
-        <v>4.7619047619047623E-2</v>
-      </c>
-      <c r="F16" s="16">
+      <c r="E16" s="11">
+        <v>4.7619047619047603E-2</v>
+      </c>
+      <c r="F16" s="7">
         <v>1</v>
       </c>
-      <c r="G16" s="16">
+      <c r="G16" s="7">
         <v>9.9999999999999867E-2</v>
       </c>
-      <c r="H16" s="16">
+      <c r="H16" s="7">
         <v>3.1250000000000167E-2</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="7">
         <v>0.95238095238095211</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E17" s="11">
         <v>0</v>
       </c>
-      <c r="F17" s="16">
+      <c r="F17" s="7">
         <v>1</v>
       </c>
-      <c r="G17" s="16">
+      <c r="G17" s="7">
         <v>1E+30</v>
       </c>
-      <c r="H17" s="16">
+      <c r="H17" s="7">
         <v>4.7619047619047866E-2</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="8">
         <v>1</v>
       </c>
-      <c r="E18" s="21">
+      <c r="E18" s="12">
         <v>4.7619047619047616E-2</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="8">
         <v>1</v>
       </c>
-      <c r="G18" s="17">
+      <c r="G18" s="8">
         <v>1.9230769230769332E-2</v>
       </c>
-      <c r="H18" s="17">
+      <c r="H18" s="8">
         <v>9.0909090909090801E-2</v>
       </c>
     </row>

</xml_diff>